<commit_message>
final edits before upload
</commit_message>
<xml_diff>
--- a/documentation/780M_980_Intel_speed_results.xlsx
+++ b/documentation/780M_980_Intel_speed_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="140" windowWidth="47200" windowHeight="27440" tabRatio="500"/>
+    <workbookView xWindow="4900" yWindow="-20" windowWidth="47200" windowHeight="27440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="780M_980_Intel_results.txt" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J77" sqref="J77"/>
     </sheetView>
   </sheetViews>
@@ -2495,8 +2495,12 @@
       <c r="H204" s="1"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A9:E9"/>
     <mergeCell ref="A68:F68"/>
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A72:D72"/>
@@ -2505,11 +2509,6 @@
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A9:E9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>